<commit_message>
Partial update to quad focusing
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/FocusQuadrupole.xlsx
+++ b/21-Spreads4Tests/FocusQuadrupole.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longkr/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB625E3-09B4-AF4D-B10A-88A3E8A26E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07CB25F-8546-2244-92E4-F92923BFEA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15660" yWindow="0" windowWidth="22740" windowHeight="21600" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Focus quad test sheet:</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Brho</t>
-  </si>
-  <si>
-    <t>Tm</t>
   </si>
   <si>
     <t>Transfer matrix</t>
@@ -239,9 +236,6 @@
     </r>
   </si>
   <si>
-    <t>Br</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -260,9 +254,6 @@
       </rPr>
       <t>r</t>
     </r>
-  </si>
-  <si>
-    <t>r</t>
   </si>
   <si>
     <t>charge</t>
@@ -585,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -613,42 +604,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -680,20 +643,40 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,9 +695,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -752,7 +735,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -858,7 +841,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1000,7 +983,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1008,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:E32"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1019,112 +1002,101 @@
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="H2" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="27"/>
-      <c r="G2"/>
-      <c r="H2" s="28" t="s">
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-    </row>
-    <row r="3" spans="1:13" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="32">
+      <c r="B3" s="22">
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>7</v>
+      <c r="D3" s="25" t="s">
+        <v>6</v>
       </c>
       <c r="E3">
         <v>0.1</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3" s="35" t="s">
         <v>7</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>6</v>
       </c>
       <c r="I3">
         <v>0.1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:13" s="20" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="32">
+        <v>25</v>
+      </c>
+      <c r="B4" s="22">
         <f>I10+B3</f>
         <v>958.27208815999995</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>9</v>
+      <c r="D4" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4" s="35" t="s">
-        <v>35</v>
+        <v>9</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="I4">
         <f>E7</f>
         <v>153.93033817521612</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-    </row>
-    <row r="5" spans="1:13" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="22">
         <f>SQRT(B4^2 -I10^ 2)</f>
         <v>194.75852619692921</v>
       </c>
@@ -1132,26 +1104,22 @@
         <v>2</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="36"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="9"/>
-      <c r="G5"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="1:13" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>28</v>
+      <c r="H5" s="29"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="33"/>
+    </row>
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="B6">
         <f>B5/I10</f>
         <v>0.20757148022900346</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="31" t="s">
         <v>3</v>
       </c>
       <c r="E6">
@@ -1159,255 +1127,194 @@
         <v>0.64964451573004278</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6"/>
       <c r="H6" s="12"/>
-      <c r="I6"/>
       <c r="J6" s="6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:13" s="20" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>30</v>
+    </row>
+    <row r="7" spans="1:12" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>28</v>
       </c>
       <c r="B7">
         <f>B5/B4</f>
         <v>0.20323927682260837</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="35" t="s">
-        <v>35</v>
+      <c r="D7" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="E7">
         <f>E4/E6</f>
         <v>153.93033817521612</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="44">
+        <v>10</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1">
         <f>I4*E6</f>
         <v>100</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7"/>
+        <v>9</v>
+      </c>
       <c r="L7">
         <f>I7-E4</f>
         <v>0</v>
       </c>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" s="8">
         <v>1</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="38"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
-      <c r="G8"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
       <c r="J8" s="9"/>
-      <c r="K8"/>
       <c r="L8">
         <f>E7-I4</f>
         <v>0</v>
       </c>
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9"/>
-      <c r="C9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9" s="41"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="13"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="1:13" s="20" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
-      <c r="G10"/>
+    </row>
+    <row r="10" spans="1:12" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
       <c r="H10" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10" s="11">
         <v>938.27208815999995</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11">
-        <f>B4+B5*B18</f>
-        <v>1095.7387238030083</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11" s="33" t="s">
-        <v>37</v>
+        <f>B4+B5*B30</f>
+        <v>1055.6513512584645</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="E11">
-        <f>SQRT(1+(2*B32/B7) + B32^2)</f>
+        <f>SQRT(1+(2*B30/B7) + B30^2)</f>
         <v>2.4840106257623371</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11"/>
       <c r="H11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="11">
         <v>299792458</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:13" s="20" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="22">
         <f>SQRT(B11^2 -I10^ 2)</f>
-        <v>565.94066775707006</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="45">
+        <v>483.78224853098436</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12">
         <f>SQRT(E7/E11)</f>
         <v>7.8720054683538221</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12"/>
+        <v>11</v>
+      </c>
       <c r="H12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12">
         <f>1/I11</f>
         <v>3.3356409519815204E-9</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="45">
-        <f>B12*I13/1000</f>
-        <v>1.8877748677622506</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13">
         <f>E12*E3</f>
         <v>0.78720054683538221</v>
       </c>
       <c r="F13" s="6"/>
-      <c r="G13"/>
       <c r="H13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13" s="8">
         <f>I12*1000000000</f>
         <v>3.3356409519815204</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:13" s="20" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="8">
-        <f>B13/E3</f>
-        <v>18.877748677622506</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>41</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="35"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="E14" s="8">
         <f>E12*E11</f>
         <v>19.554145229450118</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-    </row>
-    <row r="15" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D16" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="3">
         <f>COS(E13)</f>
@@ -1431,7 +1338,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="51">
+      <c r="B19" s="36">
         <f>-SIN(E13)*E14</f>
         <v>-13.851767538806278</v>
       </c>
@@ -1439,13 +1346,13 @@
         <f>COS(E13)</f>
         <v>0.70583115577702338</v>
       </c>
-      <c r="D19" s="45">
-        <v>0</v>
-      </c>
-      <c r="E19" s="45">
-        <v>0</v>
-      </c>
-      <c r="F19" s="45">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" s="6">
@@ -1456,7 +1363,7 @@
       <c r="B20" s="12">
         <v>0</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" s="3">
@@ -1467,7 +1374,7 @@
         <f>SINH(E13)/E14</f>
         <v>4.454604468864936E-2</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20">
         <v>0</v>
       </c>
       <c r="G20" s="6">
@@ -1478,10 +1385,10 @@
       <c r="B21" s="12">
         <v>0</v>
       </c>
-      <c r="C21" s="45">
-        <v>0</v>
-      </c>
-      <c r="D21" s="51">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="36">
         <f>SINH(E13)*E14</f>
         <v>17.032830365379439</v>
       </c>
@@ -1489,7 +1396,7 @@
         <f>COSH(E13)</f>
         <v>1.326176919807601</v>
       </c>
-      <c r="F21" s="48">
+      <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" s="6">
@@ -1500,13 +1407,13 @@
       <c r="B22" s="12">
         <v>0</v>
       </c>
-      <c r="C22" s="45">
-        <v>0</v>
-      </c>
-      <c r="D22" s="45">
-        <v>0</v>
-      </c>
-      <c r="E22" s="48">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>0</v>
       </c>
       <c r="F22" s="3">
@@ -1518,7 +1425,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="51">
+      <c r="B23" s="36">
         <v>0</v>
       </c>
       <c r="C23" s="8">
@@ -1530,119 +1437,119 @@
       <c r="E23" s="8">
         <v>0</v>
       </c>
-      <c r="F23" s="51">
+      <c r="F23" s="36">
         <v>0</v>
       </c>
       <c r="G23" s="9">
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="14">
+        <f t="array" ref="E25:E30">MMULT(B18:G23,B25:B30)</f>
+        <v>0.35653823743812263</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="14">
+        <f>B$25*B18+B$26*C18+B$27*D18+B$28*E18+B$29*F18+B$30*G18</f>
+        <v>0.35653823743812263</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="14">
+        <f>E25-H25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="15">
+        <v>-6.8553006538254371</v>
+      </c>
+      <c r="H26" s="15">
+        <f>B$25*B19+B$26*C19+B$27*D19+B$28*E19+B$29*F19+B$30*G19</f>
+        <v>-6.8553006538254371</v>
+      </c>
+      <c r="K26" s="15">
+        <f t="shared" ref="K26:K30" si="0">E26-H26</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="14">
-        <f t="array" ref="E27:E32">MMULT(B18:G23,B27:B32)</f>
-        <v>0.35653823743812263</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="14">
-        <f>B$27*B18+B$28*C18+B$29*D18+B$30*E18+B$31*F18+B$32*G18</f>
-        <v>0.35653823743812263</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K27" s="14">
-        <f>E27-H27</f>
+      <c r="B27" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="E27" s="15">
+        <v>-0.40676228488001021</v>
+      </c>
+      <c r="H27" s="15">
+        <f>B$25*B20+B$26*C20+B$27*D20+B$28*E20+B$29*F20+B$30*G20</f>
+        <v>-0.40676228488001021</v>
+      </c>
+      <c r="K27" s="15">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28" s="15">
-        <v>0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="E28" s="15">
-        <v>-6.8553006538254371</v>
+        <v>-5.3750844935753515</v>
       </c>
       <c r="H28" s="15">
-        <f t="shared" ref="H28:H32" si="0">B$27*B19+B$28*C19+B$29*D19+B$30*E19+B$31*F19+B$32*G19</f>
-        <v>-6.8553006538254371</v>
+        <f>B$25*B21+B$26*C21+B$27*D21+B$28*E21+B$29*F21+B$30*G21</f>
+        <v>-5.3750844935753515</v>
       </c>
       <c r="K28" s="15">
-        <f t="shared" ref="K28:K32" si="1">E28-H28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29" s="15">
-        <v>-0.3</v>
+        <v>0.1</v>
       </c>
       <c r="E29" s="15">
-        <v>-0.40676228488001021</v>
+        <v>1.2604719289064259</v>
       </c>
       <c r="H29" s="15">
+        <f>B$25*B22+B$26*C22+B$27*D22+B$28*E22+B$29*F22+B$30*G22</f>
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="K29" s="15">
         <f t="shared" si="0"/>
-        <v>-0.40676228488001021</v>
-      </c>
-      <c r="K29" s="15">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="15">
-        <v>-0.2</v>
-      </c>
-      <c r="E30" s="15">
-        <v>-5.3750844935753515</v>
-      </c>
-      <c r="H30" s="15">
+      <c r="B30" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="16">
+        <f>B$25*B23+B$26*C23+B$27*D23+B$28*E23+B$29*F23+B$30*G23</f>
+        <v>0.5</v>
+      </c>
+      <c r="K30" s="16">
         <f t="shared" si="0"/>
-        <v>-5.3750844935753515</v>
-      </c>
-      <c r="K30" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="49">
-        <v>0.1</v>
-      </c>
-      <c r="E31" s="15">
-        <v>1.2604719289064259</v>
-      </c>
-      <c r="H31" s="15">
-        <f t="shared" si="0"/>
-        <v>1.2604719289064259</v>
-      </c>
-      <c r="K31" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="E32" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="H32" s="16">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="K32" s="16">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Comtinued edits to quads
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/FocusQuadrupole.xlsx
+++ b/21-Spreads4Tests/FocusQuadrupole.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07CB25F-8546-2244-92E4-F92923BFEA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6071251B-5277-B240-94C9-08860B05893E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
-  <si>
-    <t>Focus quad test sheet:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
   <si>
     <t>p</t>
   </si>
@@ -284,6 +281,12 @@
   </si>
   <si>
     <t>D*sqrt(k/D)</t>
+  </si>
+  <si>
+    <t>Focus quad test sheet: reference particle and dispersion</t>
+  </si>
+  <si>
+    <t>Focus quad test sheet: no reference particle</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -572,11 +575,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -619,7 +659,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -677,6 +716,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,136 +1035,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
+      <c r="L1" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="38"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="19"/>
       <c r="E2" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="20"/>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
+      <c r="L2" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="20"/>
+    </row>
+    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>23</v>
-      </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
-    </row>
-    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>24</v>
       </c>
       <c r="B3" s="22">
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>5</v>
       </c>
       <c r="E3">
         <v>0.1</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="25" t="s">
         <v>6</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>5</v>
       </c>
       <c r="I3">
         <v>0.1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="20" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="22">
+        <v>20</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>0.1</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="22">
         <f>I10+B3</f>
         <v>958.27208815999995</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="I4">
         <f>E7</f>
         <v>153.93033817521612</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="22">
+        <f>I10+M3</f>
+        <v>958.27208815999995</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="22">
         <f>SQRT(B4^2 -I10^ 2)</f>
         <v>194.75852619692921</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="26"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>27</v>
+      <c r="H5" s="28"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="32"/>
+      <c r="L5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="22">
+        <f>SQRT(M4^2 -I10^ 2)</f>
+        <v>194.75852619692921</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="B6">
         <f>B5/I10</f>
         <v>0.20757148022900346</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="31" t="s">
-        <v>3</v>
+      <c r="D6" s="30" t="s">
+        <v>2</v>
       </c>
       <c r="E6">
         <f>B5*I13/1000</f>
@@ -1129,179 +1239,282 @@
       <c r="F6" s="6"/>
       <c r="H6" s="12"/>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>28</v>
+      <c r="L6" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6">
+        <f>M5/I10</f>
+        <v>0.20757148022900346</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f>M12*I13/1000</f>
+        <v>0.65600755638185027</v>
+      </c>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>27</v>
       </c>
       <c r="B7">
         <f>B5/B4</f>
         <v>0.20323927682260837</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="25" t="s">
-        <v>32</v>
+      <c r="D7" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="E7">
         <f>E4/E6</f>
         <v>153.93033817521612</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="I7" s="1">
         <f>I4*E6</f>
         <v>100</v>
       </c>
       <c r="J7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7">
+        <f>M5/M4</f>
+        <v>0.20323927682260837</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7">
+        <f>P4/P6</f>
+        <v>152.43726848443768</v>
+      </c>
+      <c r="Q7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L7">
-        <f>I7-E4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8">
         <v>1</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="28"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="30"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="29"/>
       <c r="J8" s="9"/>
-      <c r="L8">
-        <f>E7-I4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="9"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
-      <c r="H9" s="31"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:12" ht="20" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
+    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
       <c r="H10" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" s="11">
         <v>938.27208815999995</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="41"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <f>B4+B5*B30</f>
-        <v>1055.6513512584645</v>
+        <v>958.66160521239385</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11">
         <f>SQRT(1+(2*B30/B7) + B30^2)</f>
-        <v>2.4840106257623371</v>
+        <v>1.0097946499935522</v>
       </c>
       <c r="F11" s="6"/>
       <c r="H11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="11">
         <v>299792458</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="45">
+        <f>M4+M5*B30</f>
+        <v>958.66160521239385</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="22">
         <f>SQRT(B11^2 -I10^ 2)</f>
-        <v>483.78224853098436</v>
+        <v>196.66611779428848</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12">
         <f>SQRT(E7/E11)</f>
-        <v>7.8720054683538221</v>
+        <v>12.346548849149624</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12">
         <f>1/I11</f>
         <v>3.3356409519815204E-9</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
+        <v>17</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="46">
+        <f>SQRT(M11^2 -I10^ 2)</f>
+        <v>196.66611779428848</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12">
+        <f>SQRT(P7/P11)</f>
+        <v>12.346548849149615</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="33"/>
       <c r="C13" s="6"/>
       <c r="D13" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13">
         <f>E12*E3</f>
-        <v>0.78720054683538221</v>
+        <v>1.2346548849149626</v>
       </c>
       <c r="F13" s="6"/>
       <c r="H13" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I13" s="8">
         <f>I12*1000000000</f>
         <v>3.3356409519815204</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="L13" s="33"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13">
+        <f>P12*P3</f>
+        <v>1.2346548849149617</v>
+      </c>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="34"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="28" t="s">
-        <v>38</v>
+      <c r="D14" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="E14" s="8">
         <f>E12*E11</f>
-        <v>19.554145229450118</v>
+        <v>12.467478973755339</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="P14" s="8">
+        <f>P12*P11</f>
+        <v>12.346548849149615</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -1309,20 +1522,20 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D16" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="3">
         <f>COS(E13)</f>
-        <v>0.70583115577702338</v>
+        <v>0.32984694494413863</v>
       </c>
       <c r="C18" s="4">
         <f>SIN(E13)/E14</f>
-        <v>3.622659549610921E-2</v>
+        <v>7.5719752611650232E-2</v>
       </c>
       <c r="D18" s="11">
         <v>0</v>
@@ -1336,15 +1549,38 @@
       <c r="G18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="36">
+      <c r="L18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3">
+        <f>COS(P13)</f>
+        <v>0.32984694494413946</v>
+      </c>
+      <c r="N18" s="4">
+        <f>SIN(P13)/P14</f>
+        <v>7.6461401086079725E-2</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0</v>
+      </c>
+      <c r="P18" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B19" s="35">
         <f>-SIN(E13)*E14</f>
-        <v>-13.851767538806278</v>
+        <v>-11.769729326531085</v>
       </c>
       <c r="C19" s="9">
         <f>COS(E13)</f>
-        <v>0.70583115577702338</v>
+        <v>0.32984694494413863</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1358,8 +1594,29 @@
       <c r="G19" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="1"/>
+      <c r="M19" s="35">
+        <f>-SIN(P13)*P14</f>
+        <v>-11.655567126055011</v>
+      </c>
+      <c r="N19" s="9">
+        <f>COS(P13)</f>
+        <v>0.32984694494413946</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B20" s="12">
         <v>0</v>
       </c>
@@ -1368,11 +1625,11 @@
       </c>
       <c r="D20" s="3">
         <f>COSH(E13)</f>
-        <v>1.326176919807601</v>
+        <v>1.8640636201512468</v>
       </c>
       <c r="E20" s="4">
         <f>SINH(E13)/E14</f>
-        <v>4.454604468864936E-2</v>
+        <v>0.1261785540051294</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1380,21 +1637,42 @@
       <c r="G20" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="1"/>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <f>COSH(P13)</f>
+        <v>1.8640636201512455</v>
+      </c>
+      <c r="P20" s="4">
+        <f>SINH(P13)/P14</f>
+        <v>0.12741442877830209</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B21" s="12">
         <v>0</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="35">
         <f>SINH(E13)*E14</f>
-        <v>17.032830365379439</v>
+        <v>19.612946110246039</v>
       </c>
       <c r="E21" s="9">
         <f>COSH(E13)</f>
-        <v>1.326176919807601</v>
+        <v>1.8640636201512468</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1402,8 +1680,29 @@
       <c r="G21" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="1"/>
+      <c r="M21" s="12">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="35">
+        <f>SINH(P13)*P14</f>
+        <v>19.4227074884693</v>
+      </c>
+      <c r="P21" s="9">
+        <f>COSH(P13)</f>
+        <v>1.8640636201512455</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B22" s="12">
         <v>0</v>
       </c>
@@ -1423,9 +1722,29 @@
         <f>E3/B6^2</f>
         <v>2.3209438578128516</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="36">
+      <c r="L22" s="1"/>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4">
+        <f>P3/M6^2</f>
+        <v>2.3209438578128516</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B23" s="35">
         <v>0</v>
       </c>
       <c r="C23" s="8">
@@ -1437,124 +1756,294 @@
       <c r="E23" s="8">
         <v>0</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F23" s="35">
         <v>0</v>
       </c>
       <c r="G23" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="1"/>
+      <c r="M23" s="35">
+        <v>0</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0</v>
+      </c>
+      <c r="O23" s="8">
+        <v>0</v>
+      </c>
+      <c r="P23" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="35">
+        <v>0</v>
+      </c>
+      <c r="R23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="14">
+        <f t="array" ref="D25:D30">MMULT(B18:G23,B25:B30)</f>
+        <v>1.7249544773323435E-2</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="14">
-        <f t="array" ref="E25:E30">MMULT(B18:G23,B25:B30)</f>
-        <v>0.35653823743812263</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>14</v>
+      <c r="F25" s="14">
+        <f>B$25*B18+B$26*C18+B$27*D18+B$28*E18+B$29*F18+B$30*G18</f>
+        <v>1.7249544773323435E-2</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="H25" s="14">
-        <f>B$25*B18+B$26*C18+B$27*D18+B$28*E18+B$29*F18+B$30*G18</f>
-        <v>0.35653823743812263</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" s="14">
-        <f>E25-H25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <f>D25-F25</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="47">
+        <f>B25</f>
+        <v>0.05</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="14">
+        <f t="array" ref="O25:O30">MMULT(M18:R23,M25:M30)</f>
+        <v>1.7256961258067773E-2</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25" s="14">
+        <f>M$25*M18+M$26*N18+M$27*O18+M$28*P18+M$29*Q18+M$30*R18</f>
+        <v>1.7256961258067773E-2</v>
+      </c>
+      <c r="R25" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="S25" s="14">
+        <f>O25-Q25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B26" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="E26" s="15">
-        <v>-6.8553006538254371</v>
+        <v>0.01</v>
+      </c>
+      <c r="D26" s="15">
+        <v>-0.58518799687711287</v>
+      </c>
+      <c r="F26" s="15">
+        <f>B$25*B19+B$26*C19+B$27*D19+B$28*E19+B$29*F19+B$30*G19</f>
+        <v>-0.58518799687711287</v>
       </c>
       <c r="H26" s="15">
-        <f>B$25*B19+B$26*C19+B$27*D19+B$28*E19+B$29*F19+B$30*G19</f>
-        <v>-6.8553006538254371</v>
-      </c>
-      <c r="K26" s="15">
-        <f t="shared" ref="K26:K30" si="0">E26-H26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <f>D26-F26</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="48">
+        <f t="shared" ref="M26:M30" si="0">B26</f>
+        <v>0.01</v>
+      </c>
+      <c r="O26" s="15">
+        <v>-0.5794798868533092</v>
+      </c>
+      <c r="Q26" s="15">
+        <f>M$25*M19+M$26*N19+M$27*O19+M$28*P19+M$29*Q19+M$30*R19</f>
+        <v>-0.5794798868533092</v>
+      </c>
+      <c r="S26" s="15">
+        <f>O26-Q26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B27" s="15">
-        <v>-0.3</v>
-      </c>
-      <c r="E27" s="15">
-        <v>-0.40676228488001021</v>
+        <v>-0.03</v>
+      </c>
+      <c r="D27" s="15">
+        <v>-5.8445479684639992E-2</v>
+      </c>
+      <c r="F27" s="15">
+        <f>B$25*B20+B$26*C20+B$27*D20+B$28*E20+B$29*F20+B$30*G20</f>
+        <v>-5.8445479684639992E-2</v>
       </c>
       <c r="H27" s="15">
-        <f>B$25*B20+B$26*C20+B$27*D20+B$28*E20+B$29*F20+B$30*G20</f>
-        <v>-0.40676228488001021</v>
-      </c>
-      <c r="K27" s="15">
+        <f>D27-F27</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="48">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-0.03</v>
+      </c>
+      <c r="O27" s="15">
+        <v>-5.8470197180103406E-2</v>
+      </c>
+      <c r="Q27" s="15">
+        <f>M$25*M20+M$26*N20+M$27*O20+M$28*P20+M$29*Q20+M$30*R20</f>
+        <v>-5.8470197180103406E-2</v>
+      </c>
+      <c r="S27" s="15">
+        <f>O27-Q27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B28" s="15">
-        <v>-0.2</v>
-      </c>
-      <c r="E28" s="15">
-        <v>-5.3750844935753515</v>
+        <v>-0.02</v>
+      </c>
+      <c r="D28" s="15">
+        <v>-0.62566965571040611</v>
+      </c>
+      <c r="F28" s="15">
+        <f>B$25*B21+B$26*C21+B$27*D21+B$28*E21+B$29*F21+B$30*G21</f>
+        <v>-0.62566965571040611</v>
       </c>
       <c r="H28" s="15">
-        <f>B$25*B21+B$26*C21+B$27*D21+B$28*E21+B$29*F21+B$30*G21</f>
-        <v>-5.3750844935753515</v>
-      </c>
-      <c r="K28" s="15">
+        <f>D28-F28</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="48">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+        <v>-0.02</v>
+      </c>
+      <c r="O28" s="15">
+        <v>-0.61996249705710393</v>
+      </c>
+      <c r="Q28" s="15">
+        <f>M$25*M21+M$26*N21+M$27*O21+M$28*P21+M$29*Q21+M$30*R21</f>
+        <v>-0.61996249705710393</v>
+      </c>
+      <c r="S28" s="15">
+        <f>O28-Q28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B29" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="E29" s="15">
-        <v>1.2604719289064259</v>
+        <v>0.01</v>
+      </c>
+      <c r="D29" s="15">
+        <v>1.4641887715625704E-2</v>
+      </c>
+      <c r="F29" s="15">
+        <f>B$25*B22+B$26*C22+B$27*D22+B$28*E22+B$29*F22+B$30*G22</f>
+        <v>1.4641887715625704E-2</v>
       </c>
       <c r="H29" s="15">
-        <f>B$25*B22+B$26*C22+B$27*D22+B$28*E22+B$29*F22+B$30*G22</f>
-        <v>1.2604719289064259</v>
-      </c>
-      <c r="K29" s="15">
+        <f>D29-F29</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="48">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+      <c r="O29" s="15">
+        <v>1.4641887715625704E-2</v>
+      </c>
+      <c r="Q29" s="15">
+        <f>M$25*M22+M$26*N22+M$27*O22+M$28*P22+M$29*Q22+M$30*R22</f>
+        <v>1.4641887715625704E-2</v>
+      </c>
+      <c r="S29" s="15">
+        <f>O29-Q29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B30" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="E30" s="16">
-        <v>0.5</v>
+        <v>2E-3</v>
+      </c>
+      <c r="D30" s="16">
+        <v>2E-3</v>
+      </c>
+      <c r="F30" s="16">
+        <f>B$25*B23+B$26*C23+B$27*D23+B$28*E23+B$29*F23+B$30*G23</f>
+        <v>2E-3</v>
       </c>
       <c r="H30" s="16">
-        <f>B$25*B23+B$26*C23+B$27*D23+B$28*E23+B$29*F23+B$30*G23</f>
-        <v>0.5</v>
-      </c>
-      <c r="K30" s="16">
+        <f>D30-F30</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2E-3</v>
+      </c>
+      <c r="O30" s="16">
+        <v>2E-3</v>
+      </c>
+      <c r="Q30" s="16">
+        <f>M$25*M23+M$26*N23+M$27*O23+M$28*P23+M$29*Q23+M$30*R23</f>
+        <v>2E-3</v>
+      </c>
+      <c r="S30" s="16">
+        <f>O30-Q30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <f>(B25^2+B27^2)/(2*E11^2)</f>
+        <v>1.6671811470728866E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G35" s="22">
+        <f>B3</f>
+        <v>20</v>
+      </c>
+      <c r="H35">
+        <f>0.02*G35</f>
+        <v>0.4</v>
+      </c>
+      <c r="I35">
+        <f>G35+H35</f>
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <f>I10+G35</f>
+        <v>958.27208815999995</v>
+      </c>
+      <c r="I36">
+        <f>I10+I35</f>
+        <v>958.67208815999993</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <f>(I36-G36)/B5</f>
+        <v>2.0538253590783443E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="H2:J2"/>

</xml_diff>